<commit_message>
Profiling + automatacelular multithread
</commit_message>
<xml_diff>
--- a/BSP.xlsx
+++ b/BSP.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logan\Desktop\Projects\TFG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8B17F6CE-933A-40D7-AF04-A8ADE9DCECFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB8AA72-9996-40BB-B832-9170112EE436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BSP" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,25 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>memory</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -885,7 +902,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -917,7 +934,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -1024,7 +1041,515 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Consumo en Memoria de BSP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="53975" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000">
+                    <a:alpha val="52000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>BSP!$A$10:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BSP!$A$11:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>134.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>230.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>341.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-802A-4F3F-A0D4-665A34A7056D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1791027055"/>
+        <c:axId val="1791026575"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1791027055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Número</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-ES" baseline="0"/>
+                  <a:t> de celdas totales del mapa</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-ES"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1791026575"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1791026575"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>KB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1791027055"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1580,20 +2105,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1613,6 +2654,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>716280</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB6D181D-C3A4-59D1-8F96-55E7988DFF86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1937,16 +3014,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>50</v>
       </c>
@@ -1983,8 +3060,11 @@
       <c r="L1">
         <v>600</v>
       </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2020,6 +3100,95 @@
       </c>
       <c r="L2">
         <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>50</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>150</v>
+      </c>
+      <c r="D10">
+        <v>200</v>
+      </c>
+      <c r="E10">
+        <v>250</v>
+      </c>
+      <c r="F10">
+        <v>300</v>
+      </c>
+      <c r="G10">
+        <v>350</v>
+      </c>
+      <c r="H10">
+        <v>400</v>
+      </c>
+      <c r="I10">
+        <v>450</v>
+      </c>
+      <c r="J10">
+        <v>500</v>
+      </c>
+      <c r="K10">
+        <v>550</v>
+      </c>
+      <c r="L10">
+        <v>600</v>
+      </c>
+      <c r="M10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>55.6</v>
+      </c>
+      <c r="C11">
+        <v>134.30000000000001</v>
+      </c>
+      <c r="D11">
+        <v>230.4</v>
+      </c>
+      <c r="E11">
+        <v>341.2</v>
+      </c>
+      <c r="F11">
+        <v>500</v>
+      </c>
+      <c r="G11">
+        <v>700</v>
+      </c>
+      <c r="H11">
+        <v>900</v>
+      </c>
+      <c r="I11">
+        <v>1200</v>
+      </c>
+      <c r="J11">
+        <v>1400</v>
+      </c>
+      <c r="K11">
+        <v>1700</v>
+      </c>
+      <c r="L11">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>